<commit_message>
US9 Test Scenario TDA
The test doc for US9 is done, please review.
</commit_message>
<xml_diff>
--- a/SimpCity US9 Test Cases.xlsx
+++ b/SimpCity US9 Test Cases.xlsx
@@ -8,21 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sem3.2-DevOps\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8D453A-6522-4C78-AED2-CFB6AB32D795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE010B40-22B0-4666-B6EF-9128D9741E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US9" sheetId="11" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
   <si>
     <t>Test Scenarios for SimpCity</t>
   </si>
@@ -213,12 +211,43 @@
     <t>The user selects the building to input in the configure menu, then enter the positon to place the building in the grid map.</t>
   </si>
   <si>
+    <t xml:space="preserve">Before: Start New Game option is selected. 
+Empty 4x4 board with the message "Turn 1" shall be displayed. 
+The confiugration menu with an option rangning from "0" to "5" should be displayed 
+Build a building option is selected -&gt; Your Choice? [option value 1 to 2] is enter
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After: 
+1.Build where? [alphabet in Caps or lower case+ number, the alphabet should range from "a" to "d" or "A" to "D" and the number should range from "1" to "4". ] </t>
+  </si>
+  <si>
+    <t>1. The building name is displayed in the board with its position being the input indicated by the user when the message "Build Where" is prompted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After: 
+2. Build where? [alphabet in Caps or lower case+ number, the alphabet should range beyond "a" to "d" or "A" to "D" and  the number is beyond "1" to "4". ] </t>
+  </si>
+  <si>
+    <t>Error in program as input validation was not done yet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After:
+3. Build where? [A combintation of not a alphabet + number is entered] </t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Mr Low</t>
+  </si>
+  <si>
     <t xml:space="preserve">1. The user enters an option value of the numeric interger either "1" to "2" when the message "Your Choice?" is prompted to the users. 
 2. Then the message "Build Where?" is prompted to the users 
 3. The user enters a valur of [alphabet in Caps or lower case+ number, the alphabet should range from "a" to "d" or "A" to "D" and the number should range from "1" to "4". ] 
 e.g. b2
-4. The user enters  [alphabet in Caps or lower case+ number, the alphabet should range beyond "a" to "d" or "A" to "D" and  the number is beyond "1" to "4". ] 
-e.g. Z1
+4. The user selects either "1" to "2" again when Your Choice?" is prompted. the the user enters [alphabet in Caps or lower case+ number, the alphabet should range beyond "a" to "d" or "A" to "D" and  the number is beyond "1" to "4". ] 
+e.g. Z5
 5. The user restart the program again
 6. The user starts a new game and enters an option value of the numeric interger either "1" to "2" when the message "Your Choice?" is prompted to the users.
 7. Then the message "Build Where?" is prompted to the users.
@@ -227,29 +256,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Before: Start New Game option is selected. 
-Empty 4x4 board with the message "Turn 1" shall be displayed. 
-The confiugration menu with an option rangning from "0" to "5" should be displayed 
-Build a building option is selected -&gt; Your Choice? [option value 1 to 2] is enter
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">After: 
-1.Build where? [alphabet in Caps or lower case+ number, the alphabet should range from "a" to "d" or "A" to "D" and the number should range from "1" to "4". ] </t>
-  </si>
-  <si>
-    <t>1. The building name is displayed in the board with its position being the input indicated by the user when the message "Build Where" is prompted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">After: 
-2. Build where? [alphabet in Caps or lower case+ number, the alphabet should range beyond "a" to "d" or "A" to "D" and  the number is beyond "1" to "4". ] </t>
-  </si>
-  <si>
-    <t>Error in program as input validation was not done yet.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">After:
-3. Build where? [A combintation of not a alphabet + number is entered] </t>
+    <t>Claris (Approved in GitHub Pull Request)</t>
   </si>
 </sst>
 </file>
@@ -949,7 +956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
@@ -1237,56 +1244,59 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1303,6 +1313,231 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2250939</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>60958</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>6420630</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>5124450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FC48F40-563C-42C0-8840-DBBBDEA62370}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18224364" y="3718558"/>
+          <a:ext cx="4158261" cy="5063492"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2249805</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>6456045</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>5066250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55E9305D-FB93-41F2-A7AB-FB773AFD0DC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18223230" y="8934449"/>
+          <a:ext cx="4217670" cy="4990051"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2632440</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>89534</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5639297</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>4934915</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F84F32F-C147-47EC-815A-FBAE438C53D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18605865" y="19349084"/>
+          <a:ext cx="3006857" cy="4833951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1546020</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1905</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>6269613</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>5163175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0D88689-1CE6-44F5-AD39-D5D6DACF274A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17512503" y="24427880"/>
+          <a:ext cx="4715973" cy="5149840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1220058</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>6571182</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>4667648</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD9027FF-626B-4B98-A795-D61FD1B81029}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17198513" y="29752247"/>
+          <a:ext cx="5354934" cy="4572505"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1604,8 +1839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50695FDC-02D5-4D73-A6D6-A012274DB30C}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1618,7 +1853,8 @@
     <col min="6" max="6" width="31.109375" style="9" customWidth="1"/>
     <col min="7" max="7" width="18" style="9" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" style="9" customWidth="1"/>
-    <col min="9" max="10" width="25.109375" style="9" customWidth="1"/>
+    <col min="9" max="9" width="112.44140625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="25.109375" style="9" customWidth="1"/>
     <col min="11" max="11" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1640,12 +1876,12 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="65"/>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="105" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="106"/>
       <c r="D2" s="24"/>
-      <c r="E2" s="108" t="s">
+      <c r="E2" s="105" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="106"/>
@@ -1654,10 +1890,10 @@
         <v>3</v>
       </c>
       <c r="I2" s="106"/>
-      <c r="J2" s="108" t="s">
+      <c r="J2" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="109"/>
+      <c r="K2" s="107"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1702,12 +1938,16 @@
       <c r="E4" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="77"/>
+      <c r="F4" s="122" t="s">
+        <v>11</v>
+      </c>
       <c r="G4" s="82"/>
       <c r="H4" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="77"/>
+      <c r="I4" s="77" t="s">
+        <v>63</v>
+      </c>
       <c r="J4" s="60" t="s">
         <v>14</v>
       </c>
@@ -1728,12 +1968,16 @@
       <c r="E5" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="97"/>
+      <c r="F5" s="97" t="s">
+        <v>62</v>
+      </c>
       <c r="G5" s="50"/>
       <c r="H5" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="55"/>
+      <c r="I5" s="55" t="s">
+        <v>62</v>
+      </c>
       <c r="J5" s="60" t="s">
         <v>20</v>
       </c>
@@ -1748,13 +1992,15 @@
         <v>17</v>
       </c>
       <c r="C6" s="87">
-        <v>44545</v>
+        <v>44538</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="85"/>
+      <c r="F6" s="87">
+        <v>44541</v>
+      </c>
       <c r="G6" s="50"/>
       <c r="H6" s="88" t="s">
         <v>19</v>
@@ -1770,20 +2016,20 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="107"/>
+      <c r="C7" s="121"/>
       <c r="D7" s="18"/>
-      <c r="E7" s="107" t="s">
+      <c r="E7" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="107"/>
+      <c r="F7" s="121"/>
       <c r="G7" s="50"/>
-      <c r="H7" s="107" t="s">
+      <c r="H7" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="107"/>
+      <c r="I7" s="121"/>
       <c r="J7"/>
       <c r="L7" s="4"/>
     </row>
@@ -1793,7 +2039,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="90" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="91" t="s">
@@ -1917,7 +2163,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="243.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="49">
         <v>1</v>
       </c>
@@ -1943,10 +2189,12 @@
         <v>40</v>
       </c>
       <c r="I14" s="21"/>
-      <c r="J14" s="25"/>
+      <c r="J14" s="25" t="s">
+        <v>40</v>
+      </c>
       <c r="K14" s="45"/>
     </row>
-    <row r="15" spans="1:12" ht="277.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="25">
         <v>2</v>
       </c>
@@ -1972,27 +2220,29 @@
         <v>40</v>
       </c>
       <c r="I15" s="21"/>
-      <c r="J15" s="25"/>
+      <c r="J15" s="25" t="s">
+        <v>40</v>
+      </c>
       <c r="K15" s="46"/>
     </row>
-    <row r="16" spans="1:12" ht="174.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="118">
+    <row r="16" spans="1:12" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="108">
         <v>3</v>
       </c>
-      <c r="B16" s="115" t="s">
+      <c r="B16" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="105" t="s">
-        <v>56</v>
+      <c r="C16" s="114" t="s">
+        <v>64</v>
       </c>
       <c r="D16" s="99" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F16" s="40"/>
-      <c r="G16" s="110" t="s">
+      <c r="G16" s="115" t="s">
         <v>39</v>
       </c>
       <c r="H16" s="43"/>
@@ -2000,63 +2250,69 @@
       <c r="J16" s="25"/>
       <c r="K16" s="47"/>
     </row>
-    <row r="17" spans="1:11" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="119"/>
-      <c r="B17" s="116"/>
-      <c r="C17" s="105"/>
+    <row r="17" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="109"/>
+      <c r="B17" s="112"/>
+      <c r="C17" s="114"/>
       <c r="D17" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="113" t="s">
+      <c r="F17" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="111"/>
+      <c r="G17" s="116"/>
       <c r="H17" s="8" t="s">
         <v>40</v>
       </c>
       <c r="I17" s="21"/>
-      <c r="J17" s="25"/>
+      <c r="J17" s="25" t="s">
+        <v>40</v>
+      </c>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="1:11" ht="165.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="119"/>
-      <c r="B18" s="116"/>
-      <c r="C18" s="105"/>
+    <row r="18" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="109"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="114"/>
       <c r="D18" s="100" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="121"/>
-      <c r="G18" s="111"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="116"/>
       <c r="H18" s="36" t="s">
         <v>43</v>
       </c>
       <c r="I18" s="21"/>
-      <c r="J18" s="25"/>
+      <c r="J18" s="25" t="s">
+        <v>40</v>
+      </c>
       <c r="K18" s="14"/>
     </row>
-    <row r="19" spans="1:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="120"/>
-      <c r="B19" s="117"/>
-      <c r="C19" s="105"/>
+    <row r="19" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="110"/>
+      <c r="B19" s="113"/>
+      <c r="C19" s="114"/>
       <c r="D19" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="114"/>
-      <c r="G19" s="112"/>
+        <v>60</v>
+      </c>
+      <c r="F19" s="120"/>
+      <c r="G19" s="117"/>
       <c r="H19" s="43" t="s">
         <v>43</v>
       </c>
       <c r="I19" s="21"/>
-      <c r="J19" s="25"/>
+      <c r="J19" s="25" t="s">
+        <v>40</v>
+      </c>
       <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -2191,19 +2447,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="B16:B19"/>
     <mergeCell ref="C16:C19"/>
     <mergeCell ref="G16:G19"/>
     <mergeCell ref="F17:F19"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="H7:I7"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 F5 I5" xr:uid="{1DFF6322-A6DF-48CD-ABC4-CF22F854B949}">
@@ -2214,5 +2470,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
US9 Test Cases System Testing Approved
Approved US9 Test cases system testing with signatures
</commit_message>
<xml_diff>
--- a/SimpCity US9 Test Cases.xlsx
+++ b/SimpCity US9 Test Cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sem3.2-DevOps\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE010B40-22B0-4666-B6EF-9128D9741E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B57FAB2-8F42-463C-B053-D3F7C4DA751A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US9" sheetId="11" r:id="rId1"/>
@@ -1241,6 +1241,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1252,51 +1297,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1839,8 +1839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50695FDC-02D5-4D73-A6D6-A012274DB30C}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1860,10 +1860,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29"/>
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="104"/>
+      <c r="C1" s="119"/>
       <c r="D1" s="68"/>
       <c r="E1" s="66"/>
       <c r="F1" s="70"/>
@@ -1876,24 +1876,24 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="65"/>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="106"/>
+      <c r="C2" s="121"/>
       <c r="D2" s="24"/>
-      <c r="E2" s="105" t="s">
+      <c r="E2" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="106"/>
+      <c r="F2" s="121"/>
       <c r="G2" s="30"/>
-      <c r="H2" s="106" t="s">
+      <c r="H2" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="106"/>
-      <c r="J2" s="105" t="s">
+      <c r="I2" s="121"/>
+      <c r="J2" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="107"/>
+      <c r="K2" s="122"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1938,7 +1938,7 @@
       <c r="E4" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="122" t="s">
+      <c r="F4" s="104" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="82"/>
@@ -1969,7 +1969,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="97" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="G5" s="50"/>
       <c r="H5" s="53" t="s">
@@ -2016,20 +2016,20 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
-      <c r="B7" s="121" t="s">
+      <c r="B7" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="121"/>
+      <c r="C7" s="105"/>
       <c r="D7" s="18"/>
-      <c r="E7" s="121" t="s">
+      <c r="E7" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="121"/>
+      <c r="F7" s="105"/>
       <c r="G7" s="50"/>
-      <c r="H7" s="121" t="s">
+      <c r="H7" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="121"/>
+      <c r="I7" s="105"/>
       <c r="J7"/>
       <c r="L7" s="4"/>
     </row>
@@ -2046,7 +2046,7 @@
         <v>26</v>
       </c>
       <c r="F8" s="92" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G8" s="56"/>
       <c r="H8" s="93" t="s">
@@ -2068,7 +2068,7 @@
         <v>24</v>
       </c>
       <c r="F9" s="90" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="G9" s="50"/>
       <c r="H9" s="94" t="s">
@@ -2226,13 +2226,13 @@
       <c r="K15" s="46"/>
     </row>
     <row r="16" spans="1:12" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="108">
+      <c r="A16" s="106">
         <v>3</v>
       </c>
-      <c r="B16" s="111" t="s">
+      <c r="B16" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="114" t="s">
+      <c r="C16" s="112" t="s">
         <v>64</v>
       </c>
       <c r="D16" s="99" t="s">
@@ -2242,7 +2242,7 @@
         <v>56</v>
       </c>
       <c r="F16" s="40"/>
-      <c r="G16" s="115" t="s">
+      <c r="G16" s="113" t="s">
         <v>39</v>
       </c>
       <c r="H16" s="43"/>
@@ -2251,19 +2251,19 @@
       <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="109"/>
-      <c r="B17" s="112"/>
-      <c r="C17" s="114"/>
+      <c r="A17" s="107"/>
+      <c r="B17" s="110"/>
+      <c r="C17" s="112"/>
       <c r="D17" s="100" t="s">
         <v>57</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="118" t="s">
+      <c r="F17" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="116"/>
+      <c r="G17" s="114"/>
       <c r="H17" s="8" t="s">
         <v>40</v>
       </c>
@@ -2274,17 +2274,17 @@
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="109"/>
-      <c r="B18" s="112"/>
-      <c r="C18" s="114"/>
+      <c r="A18" s="107"/>
+      <c r="B18" s="110"/>
+      <c r="C18" s="112"/>
       <c r="D18" s="100" t="s">
         <v>59</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="119"/>
-      <c r="G18" s="116"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="114"/>
       <c r="H18" s="36" t="s">
         <v>43</v>
       </c>
@@ -2295,17 +2295,17 @@
       <c r="K18" s="14"/>
     </row>
     <row r="19" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="110"/>
-      <c r="B19" s="113"/>
-      <c r="C19" s="114"/>
+      <c r="A19" s="108"/>
+      <c r="B19" s="111"/>
+      <c r="C19" s="112"/>
       <c r="D19" s="26" t="s">
         <v>61</v>
       </c>
       <c r="E19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="120"/>
-      <c r="G19" s="117"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="115"/>
       <c r="H19" s="43" t="s">
         <v>43</v>
       </c>
@@ -2447,6 +2447,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="H7:I7"/>
@@ -2455,11 +2460,6 @@
     <mergeCell ref="C16:C19"/>
     <mergeCell ref="G16:G19"/>
     <mergeCell ref="F17:F19"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 F5 I5" xr:uid="{1DFF6322-A6DF-48CD-ABC4-CF22F854B949}">

</xml_diff>